<commit_message>
finished the multiple regression to predice RT_Asym
</commit_message>
<xml_diff>
--- a/Analyses Scripts_R/Participant_Demographics.xlsx
+++ b/Analyses Scripts_R/Participant_Demographics.xlsx
@@ -703,7 +703,7 @@
   <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,7 +786,9 @@
       <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4">
+        <v>33756</v>
+      </c>
       <c r="D5" s="4">
         <v>41744</v>
       </c>
@@ -840,7 +842,9 @@
       <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4">
+        <v>33419</v>
+      </c>
       <c r="D9" s="4">
         <v>41754</v>
       </c>

</xml_diff>